<commit_message>
MEJORA: carga de invenatrio en upload almacen
</commit_message>
<xml_diff>
--- a/public/uploads/files/almacen_productos_alpina.xlsx
+++ b/public/uploads/files/almacen_productos_alpina.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Descargas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\alpinav2\public\uploads\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,12 +19,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>REFERENCIA</t>
   </si>
   <si>
     <t>Frutto Litteral x3 x305ml c/u EAN</t>
+  </si>
+  <si>
+    <t>Inventario Dispoible</t>
   </si>
 </sst>
 </file>
@@ -855,7 +858,7 @@
   <dimension ref="A1:F2393"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2:XFD49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,251 +875,401 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>7702001100095</v>
       </c>
+      <c r="B2">
+        <v>55</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>56</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>7702001011452</v>
       </c>
+      <c r="B4">
+        <v>57</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>7702001121748</v>
       </c>
+      <c r="B5">
+        <v>58</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>7702001121755</v>
       </c>
+      <c r="B6">
+        <v>59</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>7702001115518</v>
       </c>
+      <c r="B7">
+        <v>60</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7702001116966</v>
       </c>
+      <c r="B8">
+        <v>61</v>
+      </c>
       <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>7702001117437</v>
       </c>
+      <c r="B9">
+        <v>62</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>7702001122011</v>
       </c>
+      <c r="B10">
+        <v>63</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>7702001124763</v>
       </c>
+      <c r="B11">
+        <v>64</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>7702001012022</v>
       </c>
+      <c r="B12">
+        <v>65</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>7702001012053</v>
       </c>
+      <c r="B13">
+        <v>66</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>7702001011308</v>
       </c>
+      <c r="B14">
+        <v>67</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>7702001112388</v>
       </c>
+      <c r="B15">
+        <v>68</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>7702001101498</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>7702001101573</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>7702001102730</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>7702001010455</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>7702001104635</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>7702001010486</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>7702001012138</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>7702001121731</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>7702001106684</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>7702001121762</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>7702001127269</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>7702001012084</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>7702001012053</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>7702001041985</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>7702001106684</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>7702001027576</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>7702001025015</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>7702001010486</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>7702001104635</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>7702001010455</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>7702001102730</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>7702001101573</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>7702001101498</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>7702001044481</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>7702001112388</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>7702001011308</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>7702001012022</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>7702001044115</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>7702001041992</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>7702001117437</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>7702001116966</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>7702001115518</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>7702001041954</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>7702001029716</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>7702001011452</v>
+      </c>
+      <c r="B50">
+        <v>103</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
@@ -4452,5 +4605,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
MEJORA: ajustes de archivo
</commit_message>
<xml_diff>
--- a/public/uploads/files/almacen_productos_alpina.xlsx
+++ b/public/uploads/files/almacen_productos_alpina.xlsx
@@ -19,12 +19,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>REFERENCIA</t>
-  </si>
-  <si>
-    <t>Frutto Litteral x3 x305ml c/u EAN</t>
   </si>
   <si>
     <t>Inventario Dispoible</t>
@@ -855,10 +852,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2393"/>
+  <dimension ref="A1:F2349"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD49"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,407 +868,72 @@
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>7702001100095</v>
+        <v>7702001116966</v>
       </c>
       <c r="B2">
-        <v>55</v>
+        <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>1</v>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>7702001115518</v>
       </c>
       <c r="B3">
-        <v>56</v>
+        <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
+        <v>7702001041954</v>
+      </c>
+      <c r="B4">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>7702001029716</v>
+      </c>
+      <c r="B5">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
         <v>7702001011452</v>
       </c>
-      <c r="B4">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>7702001121748</v>
-      </c>
-      <c r="B5">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>7702001121755</v>
-      </c>
       <c r="B6">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>7702001115518</v>
-      </c>
-      <c r="B7">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>7702001116966</v>
-      </c>
-      <c r="B8">
-        <v>61</v>
-      </c>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>7702001117437</v>
-      </c>
-      <c r="B9">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>7702001122011</v>
-      </c>
-      <c r="B10">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>7702001124763</v>
-      </c>
-      <c r="B11">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
-        <v>7702001012022</v>
-      </c>
-      <c r="B12">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
-        <v>7702001012053</v>
-      </c>
-      <c r="B13">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
-        <v>7702001011308</v>
-      </c>
-      <c r="B14">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <v>7702001112388</v>
-      </c>
-      <c r="B15">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
-        <v>7702001101498</v>
-      </c>
-      <c r="B16">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
-        <v>7702001101573</v>
-      </c>
-      <c r="B17">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
-        <v>7702001102730</v>
-      </c>
-      <c r="B18">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
-        <v>7702001010455</v>
-      </c>
-      <c r="B19">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
-        <v>7702001104635</v>
-      </c>
-      <c r="B20">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
-        <v>7702001010486</v>
-      </c>
-      <c r="B21">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
-        <v>7702001012138</v>
-      </c>
-      <c r="B22">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
-        <v>7702001121731</v>
-      </c>
-      <c r="B23">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
-        <v>7702001106684</v>
-      </c>
-      <c r="B24">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
-        <v>7702001121762</v>
-      </c>
-      <c r="B25">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
-        <v>7702001127269</v>
-      </c>
-      <c r="B26">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
-        <v>7702001012084</v>
-      </c>
-      <c r="B27">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
-        <v>7702001012053</v>
-      </c>
-      <c r="B28">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
-        <v>7702001041985</v>
-      </c>
-      <c r="B29">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
-        <v>7702001106684</v>
-      </c>
-      <c r="B30">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="5">
-        <v>7702001027576</v>
-      </c>
-      <c r="B31">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="5">
-        <v>7702001025015</v>
-      </c>
-      <c r="B32">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="5">
-        <v>7702001010486</v>
-      </c>
-      <c r="B33">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="5">
-        <v>7702001104635</v>
-      </c>
-      <c r="B34">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="5">
-        <v>7702001010455</v>
-      </c>
-      <c r="B35">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="5">
-        <v>7702001102730</v>
-      </c>
-      <c r="B36">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="5">
-        <v>7702001101573</v>
-      </c>
-      <c r="B37">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="5">
-        <v>7702001101498</v>
-      </c>
-      <c r="B38">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="5">
-        <v>7702001044481</v>
-      </c>
-      <c r="B39">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="5">
-        <v>7702001112388</v>
-      </c>
-      <c r="B40">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="5">
-        <v>7702001011308</v>
-      </c>
-      <c r="B41">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="5">
-        <v>7702001012022</v>
-      </c>
-      <c r="B42">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="5">
-        <v>7702001044115</v>
-      </c>
-      <c r="B43">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="5">
-        <v>7702001041992</v>
-      </c>
-      <c r="B44">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="5">
-        <v>7702001117437</v>
-      </c>
-      <c r="B45">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="5">
-        <v>7702001116966</v>
-      </c>
-      <c r="B46">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="5">
-        <v>7702001115518</v>
-      </c>
-      <c r="B47">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="5">
-        <v>7702001041954</v>
-      </c>
-      <c r="B48">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="5">
-        <v>7702001029716</v>
-      </c>
-      <c r="B49">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="5">
-        <v>7702001011452</v>
-      </c>
-      <c r="B50">
         <v>103</v>
       </c>
     </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="2"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="2"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="2"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="2"/>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="2"/>
+    </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
     </row>
@@ -1284,26 +946,26 @@
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" s="2"/>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" s="2"/>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" s="2"/>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" s="2"/>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" s="2"/>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" s="2"/>
-    </row>
-    <row r="312" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F312" s="1"/>
+    <row r="268" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F268" s="1"/>
+    </row>
+    <row r="269" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F269" s="1"/>
+    </row>
+    <row r="270" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F270" s="1"/>
+    </row>
+    <row r="271" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F271" s="1"/>
+    </row>
+    <row r="272" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F272" s="1"/>
+    </row>
+    <row r="273" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F273" s="1"/>
+    </row>
+    <row r="274" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F274" s="1"/>
     </row>
     <row r="313" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F313" s="1"/>
@@ -1314,83 +976,241 @@
     <row r="315" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F315" s="1"/>
     </row>
-    <row r="316" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F316" s="1"/>
-    </row>
-    <row r="317" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F317" s="1"/>
-    </row>
-    <row r="318" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F318" s="1"/>
-    </row>
-    <row r="357" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="319" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F319" s="1"/>
+    </row>
+    <row r="320" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F320" s="1"/>
+    </row>
+    <row r="321" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F321" s="1"/>
+    </row>
+    <row r="322" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F322" s="1"/>
+    </row>
+    <row r="326" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F326" s="1"/>
+    </row>
+    <row r="329" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F329" s="1"/>
+    </row>
+    <row r="336" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F336" s="1"/>
+    </row>
+    <row r="337" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F337" s="1"/>
+    </row>
+    <row r="338" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F338" s="1"/>
+    </row>
+    <row r="339" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F339" s="1"/>
+    </row>
+    <row r="340" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F340" s="1"/>
+    </row>
+    <row r="341" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F341" s="1"/>
+    </row>
+    <row r="343" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F343" s="1"/>
+    </row>
+    <row r="344" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F344" s="1"/>
+    </row>
+    <row r="345" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F345" s="1"/>
+    </row>
+    <row r="346" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F346" s="1"/>
+    </row>
+    <row r="347" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F347" s="1"/>
+    </row>
+    <row r="351" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F351" s="1"/>
+    </row>
+    <row r="352" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F352" s="1"/>
+    </row>
+    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F353" s="1"/>
+    </row>
+    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A357"/>
       <c r="F357" s="1"/>
     </row>
-    <row r="358" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A358"/>
       <c r="F358" s="1"/>
     </row>
-    <row r="359" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A359"/>
       <c r="F359" s="1"/>
     </row>
-    <row r="363" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A360"/>
+      <c r="F360" s="1"/>
+    </row>
+    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A361"/>
+      <c r="F361" s="1"/>
+    </row>
+    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A362"/>
+      <c r="F362" s="1"/>
+    </row>
+    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A363"/>
       <c r="F363" s="1"/>
     </row>
-    <row r="364" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A364"/>
       <c r="F364" s="1"/>
     </row>
-    <row r="365" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A365"/>
       <c r="F365" s="1"/>
     </row>
-    <row r="366" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A366"/>
       <c r="F366" s="1"/>
     </row>
-    <row r="370" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A367"/>
+      <c r="F367" s="1"/>
+    </row>
+    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A368"/>
+      <c r="F368" s="1"/>
+    </row>
+    <row r="369" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A369"/>
+      <c r="F369" s="1"/>
+    </row>
+    <row r="370" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A370"/>
       <c r="F370" s="1"/>
     </row>
-    <row r="373" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A371"/>
+      <c r="F371" s="1"/>
+    </row>
+    <row r="372" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A372"/>
+      <c r="F372" s="1"/>
+    </row>
+    <row r="373" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A373"/>
       <c r="F373" s="1"/>
     </row>
-    <row r="380" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A374"/>
+      <c r="F374" s="1"/>
+    </row>
+    <row r="375" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A375"/>
+      <c r="F375" s="1"/>
+    </row>
+    <row r="376" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A376"/>
+      <c r="F376" s="1"/>
+    </row>
+    <row r="377" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A377"/>
+      <c r="F377" s="1"/>
+    </row>
+    <row r="378" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A378"/>
+      <c r="F378" s="1"/>
+    </row>
+    <row r="379" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A379"/>
+      <c r="F379" s="1"/>
+    </row>
+    <row r="380" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A380"/>
       <c r="F380" s="1"/>
     </row>
-    <row r="381" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A381"/>
       <c r="F381" s="1"/>
     </row>
-    <row r="382" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A382"/>
       <c r="F382" s="1"/>
     </row>
-    <row r="383" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A383"/>
       <c r="F383" s="1"/>
     </row>
-    <row r="384" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A384"/>
       <c r="F384" s="1"/>
     </row>
-    <row r="385" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A385"/>
       <c r="F385" s="1"/>
     </row>
-    <row r="387" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A386"/>
+      <c r="F386" s="1"/>
+    </row>
+    <row r="387" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A387"/>
       <c r="F387" s="1"/>
     </row>
-    <row r="388" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A388"/>
       <c r="F388" s="1"/>
     </row>
-    <row r="389" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A389"/>
       <c r="F389" s="1"/>
     </row>
-    <row r="390" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A390"/>
       <c r="F390" s="1"/>
     </row>
-    <row r="391" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A391"/>
       <c r="F391" s="1"/>
     </row>
-    <row r="395" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A392"/>
+      <c r="F392" s="1"/>
+    </row>
+    <row r="393" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A393"/>
+      <c r="F393" s="1"/>
+    </row>
+    <row r="394" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A394"/>
+      <c r="F394" s="1"/>
+    </row>
+    <row r="395" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A395"/>
       <c r="F395" s="1"/>
     </row>
-    <row r="396" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A396"/>
       <c r="F396" s="1"/>
     </row>
-    <row r="397" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A397"/>
       <c r="F397" s="1"/>
+    </row>
+    <row r="398" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A398"/>
+      <c r="F398" s="1"/>
+    </row>
+    <row r="399" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A399"/>
+      <c r="F399" s="1"/>
+    </row>
+    <row r="400" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A400"/>
+      <c r="F400" s="1"/>
     </row>
     <row r="401" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A401"/>
@@ -1692,14 +1512,6 @@
       <c r="A475"/>
       <c r="F475" s="1"/>
     </row>
-    <row r="476" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A476"/>
-      <c r="F476" s="1"/>
-    </row>
-    <row r="477" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A477"/>
-      <c r="F477" s="1"/>
-    </row>
     <row r="478" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A478"/>
       <c r="F478" s="1"/>
@@ -1854,6 +1666,7 @@
     </row>
     <row r="516" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A516"/>
+      <c r="B516" s="4"/>
       <c r="F516" s="1"/>
     </row>
     <row r="517" spans="1:6" x14ac:dyDescent="0.25">
@@ -1868,6 +1681,14 @@
       <c r="A519"/>
       <c r="F519" s="1"/>
     </row>
+    <row r="520" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A520"/>
+      <c r="F520" s="1"/>
+    </row>
+    <row r="521" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A521"/>
+      <c r="F521" s="1"/>
+    </row>
     <row r="522" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A522"/>
       <c r="F522" s="1"/>
@@ -2022,7 +1843,6 @@
     </row>
     <row r="560" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A560"/>
-      <c r="B560" s="4"/>
       <c r="F560" s="1"/>
     </row>
     <row r="561" spans="1:6" x14ac:dyDescent="0.25">
@@ -2369,192 +2189,148 @@
       <c r="A646"/>
       <c r="F646" s="1"/>
     </row>
-    <row r="647" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A647"/>
-      <c r="F647" s="1"/>
-    </row>
-    <row r="648" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A648"/>
-      <c r="F648" s="1"/>
-    </row>
-    <row r="649" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A649"/>
-      <c r="F649" s="1"/>
-    </row>
-    <row r="650" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A650"/>
-      <c r="F650" s="1"/>
-    </row>
-    <row r="651" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A651"/>
-      <c r="F651" s="1"/>
-    </row>
-    <row r="652" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A652"/>
-      <c r="F652" s="1"/>
-    </row>
-    <row r="653" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A653"/>
-      <c r="F653" s="1"/>
-    </row>
-    <row r="654" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A654"/>
-      <c r="F654" s="1"/>
-    </row>
-    <row r="655" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A655"/>
-      <c r="F655" s="1"/>
-    </row>
-    <row r="656" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A656"/>
-      <c r="F656" s="1"/>
-    </row>
-    <row r="657" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A657"/>
+    <row r="657" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F657" s="1"/>
     </row>
-    <row r="658" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A658"/>
+    <row r="658" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F658" s="1"/>
     </row>
-    <row r="659" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A659"/>
+    <row r="659" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F659" s="1"/>
     </row>
-    <row r="660" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A660"/>
+    <row r="660" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F660" s="1"/>
     </row>
-    <row r="661" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A661"/>
+    <row r="661" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F661" s="1"/>
     </row>
-    <row r="662" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A662"/>
+    <row r="662" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F662" s="1"/>
     </row>
-    <row r="663" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A663"/>
+    <row r="663" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F663" s="1"/>
     </row>
-    <row r="664" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A664"/>
+    <row r="664" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F664" s="1"/>
     </row>
-    <row r="665" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A665"/>
+    <row r="665" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F665" s="1"/>
     </row>
-    <row r="666" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A666"/>
+    <row r="666" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F666" s="1"/>
     </row>
-    <row r="667" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A667"/>
+    <row r="667" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F667" s="1"/>
     </row>
-    <row r="668" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A668"/>
+    <row r="668" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F668" s="1"/>
     </row>
-    <row r="669" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A669"/>
+    <row r="669" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F669" s="1"/>
     </row>
-    <row r="670" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A670"/>
+    <row r="670" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F670" s="1"/>
     </row>
-    <row r="671" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A671"/>
+    <row r="671" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F671" s="1"/>
     </row>
-    <row r="672" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A672"/>
+    <row r="672" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F672" s="1"/>
     </row>
-    <row r="673" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A673"/>
+    <row r="673" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F673" s="1"/>
     </row>
-    <row r="674" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A674"/>
+    <row r="674" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F674" s="1"/>
     </row>
-    <row r="675" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A675"/>
+    <row r="675" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F675" s="1"/>
     </row>
-    <row r="676" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A676"/>
+    <row r="676" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F676" s="1"/>
     </row>
-    <row r="677" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A677"/>
+    <row r="677" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F677" s="1"/>
     </row>
-    <row r="678" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A678"/>
+    <row r="678" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F678" s="1"/>
     </row>
-    <row r="679" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A679"/>
+    <row r="679" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F679" s="1"/>
     </row>
-    <row r="680" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A680"/>
+    <row r="680" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F680" s="1"/>
     </row>
-    <row r="681" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A681"/>
+    <row r="681" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F681" s="1"/>
     </row>
-    <row r="682" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A682"/>
+    <row r="682" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F682" s="1"/>
     </row>
-    <row r="683" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A683"/>
+    <row r="683" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F683" s="1"/>
     </row>
-    <row r="684" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A684"/>
+    <row r="684" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F684" s="1"/>
     </row>
-    <row r="685" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A685"/>
+    <row r="685" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F685" s="1"/>
     </row>
-    <row r="686" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A686"/>
+    <row r="686" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F686" s="1"/>
     </row>
-    <row r="687" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A687"/>
+    <row r="687" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F687" s="1"/>
     </row>
-    <row r="688" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A688"/>
+    <row r="688" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F688" s="1"/>
     </row>
-    <row r="689" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A689"/>
+    <row r="689" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F689" s="1"/>
     </row>
-    <row r="690" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A690"/>
+    <row r="690" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F690" s="1"/>
     </row>
-    <row r="701" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="691" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F691" s="1"/>
+    </row>
+    <row r="692" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F692" s="1"/>
+    </row>
+    <row r="693" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F693" s="1"/>
+    </row>
+    <row r="694" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F694" s="1"/>
+    </row>
+    <row r="695" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F695" s="1"/>
+    </row>
+    <row r="696" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F696" s="1"/>
+    </row>
+    <row r="697" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F697" s="1"/>
+    </row>
+    <row r="698" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F698" s="1"/>
+    </row>
+    <row r="699" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F699" s="1"/>
+    </row>
+    <row r="700" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F700" s="1"/>
+    </row>
+    <row r="701" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F701" s="1"/>
     </row>
-    <row r="702" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="702" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F702" s="1"/>
     </row>
-    <row r="703" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="703" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F703" s="1"/>
     </row>
-    <row r="704" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="704" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F704" s="1"/>
     </row>
     <row r="705" spans="6:6" x14ac:dyDescent="0.25">
@@ -3574,245 +3350,245 @@
     <row r="1043" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F1043" s="1"/>
     </row>
-    <row r="1044" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1044" s="1"/>
-    </row>
-    <row r="1045" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1045" s="1"/>
-    </row>
-    <row r="1046" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1046" s="1"/>
-    </row>
-    <row r="1047" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1047" s="1"/>
-    </row>
-    <row r="1048" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1048" s="1"/>
-    </row>
-    <row r="1049" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1049" s="1"/>
-    </row>
-    <row r="1050" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1050" s="1"/>
-    </row>
-    <row r="1051" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1051" s="1"/>
-    </row>
-    <row r="1052" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1052" s="1"/>
-    </row>
-    <row r="1053" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1053" s="1"/>
-    </row>
-    <row r="1054" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1054" s="1"/>
-    </row>
-    <row r="1055" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1055" s="1"/>
-    </row>
-    <row r="1056" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1056" s="1"/>
-    </row>
-    <row r="1057" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1057" s="1"/>
-    </row>
-    <row r="1058" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1058" s="1"/>
-    </row>
-    <row r="1059" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1059" s="1"/>
-    </row>
-    <row r="1060" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1060" s="1"/>
-    </row>
-    <row r="1061" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1061" s="1"/>
-    </row>
-    <row r="1062" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1062" s="1"/>
-    </row>
-    <row r="1063" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1063" s="1"/>
-    </row>
-    <row r="1064" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1064" s="1"/>
-    </row>
-    <row r="1065" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1065" s="1"/>
-    </row>
-    <row r="1066" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1066" s="1"/>
-    </row>
-    <row r="1067" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1067" s="1"/>
-    </row>
-    <row r="1068" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1068" s="1"/>
-    </row>
-    <row r="1069" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1069" s="1"/>
-    </row>
-    <row r="1070" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1070" s="1"/>
-    </row>
-    <row r="1071" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1071" s="1"/>
-    </row>
-    <row r="1072" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1072" s="1"/>
-    </row>
-    <row r="1073" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1073" s="1"/>
-    </row>
-    <row r="1074" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1074" s="1"/>
-    </row>
-    <row r="1075" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1075" s="1"/>
-    </row>
-    <row r="1076" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1076" s="1"/>
-    </row>
-    <row r="1077" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1077" s="1"/>
-    </row>
-    <row r="1078" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1078" s="1"/>
-    </row>
-    <row r="1079" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1079" s="1"/>
-    </row>
-    <row r="1080" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1080" s="1"/>
-    </row>
-    <row r="1081" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1081" s="1"/>
-    </row>
-    <row r="1082" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1082" s="1"/>
-    </row>
-    <row r="1083" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1083" s="1"/>
-    </row>
-    <row r="1084" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1084" s="1"/>
-    </row>
-    <row r="1085" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1085" s="1"/>
-    </row>
-    <row r="1086" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1086" s="1"/>
-    </row>
-    <row r="1087" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1087" s="1"/>
-    </row>
-    <row r="1230" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1230" s="1"/>
-    </row>
-    <row r="1247" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1247" s="1"/>
-    </row>
-    <row r="1261" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1261" s="1"/>
-    </row>
-    <row r="1262" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1262" s="1"/>
-    </row>
-    <row r="1263" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1263" s="1"/>
-    </row>
-    <row r="1264" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1264" s="1"/>
-    </row>
-    <row r="1266" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1266" s="1"/>
-    </row>
-    <row r="1267" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1267" s="1"/>
-    </row>
-    <row r="1268" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1268" s="1"/>
-    </row>
-    <row r="1354" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1354" s="2"/>
-    </row>
-    <row r="1355" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1355" s="2"/>
-    </row>
-    <row r="1356" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1356" s="2"/>
-    </row>
-    <row r="1357" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1357" s="2"/>
-    </row>
-    <row r="1358" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1358" s="2"/>
-    </row>
-    <row r="1359" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1359" s="2"/>
-    </row>
-    <row r="1360" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1360" s="2"/>
-    </row>
-    <row r="1361" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1361" s="2"/>
-    </row>
-    <row r="1362" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1362" s="2"/>
-    </row>
-    <row r="1363" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1363" s="2"/>
-    </row>
-    <row r="1461" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1461" s="2"/>
-    </row>
-    <row r="1462" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1462" s="2"/>
-    </row>
-    <row r="1463" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1463" s="2"/>
-    </row>
-    <row r="1464" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1464" s="2"/>
-    </row>
-    <row r="1465" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1465" s="2"/>
-    </row>
-    <row r="1466" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1466" s="2"/>
-    </row>
-    <row r="1467" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1467" s="2"/>
-    </row>
-    <row r="1468" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1468" s="2"/>
-    </row>
-    <row r="1469" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1469" s="2"/>
-    </row>
-    <row r="1470" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1470" s="2"/>
-    </row>
-    <row r="1471" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1471" s="2"/>
-    </row>
-    <row r="1472" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1472" s="2"/>
-    </row>
-    <row r="1473" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1473" s="2"/>
-    </row>
-    <row r="1474" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1474" s="2"/>
-    </row>
-    <row r="1475" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1475" s="2"/>
-    </row>
-    <row r="1476" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1476" s="2"/>
-    </row>
-    <row r="1477" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1477" s="2"/>
+    <row r="1186" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1186" s="1"/>
+    </row>
+    <row r="1203" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1203" s="1"/>
+    </row>
+    <row r="1217" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1217" s="1"/>
+    </row>
+    <row r="1218" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1218" s="1"/>
+    </row>
+    <row r="1219" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1219" s="1"/>
+    </row>
+    <row r="1220" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1220" s="1"/>
+    </row>
+    <row r="1222" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1222" s="1"/>
+    </row>
+    <row r="1223" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1223" s="1"/>
+    </row>
+    <row r="1224" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1224" s="1"/>
+    </row>
+    <row r="1310" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1310" s="2"/>
+    </row>
+    <row r="1311" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1311" s="2"/>
+    </row>
+    <row r="1312" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1312" s="2"/>
+    </row>
+    <row r="1313" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1313" s="2"/>
+    </row>
+    <row r="1314" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1314" s="2"/>
+    </row>
+    <row r="1315" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1315" s="2"/>
+    </row>
+    <row r="1316" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1316" s="2"/>
+    </row>
+    <row r="1317" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1317" s="2"/>
+    </row>
+    <row r="1318" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1318" s="2"/>
+    </row>
+    <row r="1319" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1319" s="2"/>
+    </row>
+    <row r="1417" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1417" s="2"/>
+    </row>
+    <row r="1418" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1418" s="2"/>
+    </row>
+    <row r="1419" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1419" s="2"/>
+    </row>
+    <row r="1420" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1420" s="2"/>
+    </row>
+    <row r="1421" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1421" s="2"/>
+    </row>
+    <row r="1422" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1422" s="2"/>
+    </row>
+    <row r="1423" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1423" s="2"/>
+    </row>
+    <row r="1424" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1424" s="2"/>
+    </row>
+    <row r="1425" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1425" s="2"/>
+    </row>
+    <row r="1426" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1426" s="2"/>
+    </row>
+    <row r="1427" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1427" s="2"/>
+    </row>
+    <row r="1428" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1428" s="2"/>
+    </row>
+    <row r="1429" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1429" s="2"/>
+    </row>
+    <row r="1430" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1430" s="2"/>
+    </row>
+    <row r="1431" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1431" s="2"/>
+    </row>
+    <row r="1432" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1432" s="2"/>
+    </row>
+    <row r="1433" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1433" s="2"/>
+    </row>
+    <row r="1632" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1632" s="1"/>
+    </row>
+    <row r="1633" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1633" s="1"/>
+    </row>
+    <row r="1634" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1634" s="1"/>
+    </row>
+    <row r="1635" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1635" s="1"/>
+    </row>
+    <row r="1636" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1636" s="1"/>
+    </row>
+    <row r="1637" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1637" s="1"/>
+    </row>
+    <row r="1638" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1638" s="1"/>
+    </row>
+    <row r="1639" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1639" s="1"/>
+    </row>
+    <row r="1640" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1640" s="1"/>
+    </row>
+    <row r="1641" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1641" s="1"/>
+    </row>
+    <row r="1642" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1642" s="1"/>
+    </row>
+    <row r="1643" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1643" s="1"/>
+    </row>
+    <row r="1644" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1644" s="1"/>
+    </row>
+    <row r="1645" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1645" s="1"/>
+    </row>
+    <row r="1646" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1646" s="1"/>
+    </row>
+    <row r="1647" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1647" s="1"/>
+    </row>
+    <row r="1648" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1648" s="1"/>
+    </row>
+    <row r="1649" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1649" s="1"/>
+    </row>
+    <row r="1650" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1650" s="1"/>
+    </row>
+    <row r="1651" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1651" s="1"/>
+    </row>
+    <row r="1652" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1652" s="1"/>
+    </row>
+    <row r="1653" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1653" s="1"/>
+    </row>
+    <row r="1654" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1654" s="1"/>
+    </row>
+    <row r="1655" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1655" s="1"/>
+    </row>
+    <row r="1656" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1656" s="1"/>
+    </row>
+    <row r="1657" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1657" s="1"/>
+    </row>
+    <row r="1658" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1658" s="1"/>
+    </row>
+    <row r="1659" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1659" s="1"/>
+    </row>
+    <row r="1660" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1660" s="1"/>
+    </row>
+    <row r="1661" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1661" s="1"/>
+    </row>
+    <row r="1662" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1662" s="1"/>
+    </row>
+    <row r="1663" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1663" s="1"/>
+    </row>
+    <row r="1664" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1664" s="1"/>
+    </row>
+    <row r="1665" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1665" s="1"/>
+    </row>
+    <row r="1666" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1666" s="1"/>
+    </row>
+    <row r="1667" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1667" s="1"/>
+    </row>
+    <row r="1668" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1668" s="1"/>
+    </row>
+    <row r="1669" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1669" s="1"/>
+    </row>
+    <row r="1670" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1670" s="1"/>
+    </row>
+    <row r="1671" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1671" s="1"/>
+    </row>
+    <row r="1672" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1672" s="1"/>
+    </row>
+    <row r="1673" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1673" s="1"/>
+    </row>
+    <row r="1674" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1674" s="1"/>
+    </row>
+    <row r="1675" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1675" s="1"/>
     </row>
     <row r="1676" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F1676" s="1"/>
@@ -3943,9 +3719,6 @@
     <row r="1718" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F1718" s="1"/>
     </row>
-    <row r="1719" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1719" s="1"/>
-    </row>
     <row r="1720" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F1720" s="1"/>
     </row>
@@ -4075,6 +3848,9 @@
     <row r="1762" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F1762" s="1"/>
     </row>
+    <row r="1763" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1763" s="1"/>
+    </row>
     <row r="1764" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F1764" s="1"/>
     </row>
@@ -4114,66 +3890,6 @@
     <row r="1776" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F1776" s="1"/>
     </row>
-    <row r="1777" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1777" s="1"/>
-    </row>
-    <row r="1778" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1778" s="1"/>
-    </row>
-    <row r="1779" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1779" s="1"/>
-    </row>
-    <row r="1780" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1780" s="1"/>
-    </row>
-    <row r="1781" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1781" s="1"/>
-    </row>
-    <row r="1782" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1782" s="1"/>
-    </row>
-    <row r="1783" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1783" s="1"/>
-    </row>
-    <row r="1784" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1784" s="1"/>
-    </row>
-    <row r="1785" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1785" s="1"/>
-    </row>
-    <row r="1786" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1786" s="1"/>
-    </row>
-    <row r="1787" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1787" s="1"/>
-    </row>
-    <row r="1788" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1788" s="1"/>
-    </row>
-    <row r="1789" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1789" s="1"/>
-    </row>
-    <row r="1790" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1790" s="1"/>
-    </row>
-    <row r="1791" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1791" s="1"/>
-    </row>
-    <row r="1792" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1792" s="1"/>
-    </row>
-    <row r="1793" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1793" s="1"/>
-    </row>
-    <row r="1794" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1794" s="1"/>
-    </row>
-    <row r="1795" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1795" s="1"/>
-    </row>
-    <row r="1796" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1796" s="1"/>
-    </row>
     <row r="1797" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F1797" s="1"/>
     </row>
@@ -4234,374 +3950,302 @@
     <row r="1816" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F1816" s="1"/>
     </row>
-    <row r="1817" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1817" s="1"/>
-    </row>
-    <row r="1818" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1818" s="1"/>
-    </row>
-    <row r="1819" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1819" s="1"/>
-    </row>
-    <row r="1820" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1820" s="1"/>
-    </row>
-    <row r="1841" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1841" s="1"/>
-    </row>
-    <row r="1842" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1842" s="1"/>
-    </row>
-    <row r="1843" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1843" s="1"/>
-    </row>
-    <row r="1844" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1844" s="1"/>
-    </row>
-    <row r="1845" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1845" s="1"/>
-    </row>
-    <row r="1846" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1846" s="1"/>
-    </row>
-    <row r="1847" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1847" s="1"/>
-    </row>
-    <row r="1848" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1848" s="1"/>
-    </row>
-    <row r="1849" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1849" s="1"/>
-    </row>
-    <row r="1850" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1850" s="1"/>
-    </row>
-    <row r="1851" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1851" s="1"/>
-    </row>
-    <row r="1852" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1852" s="1"/>
-    </row>
-    <row r="1853" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1853" s="1"/>
-    </row>
-    <row r="1854" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1854" s="1"/>
-    </row>
-    <row r="1855" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1855" s="1"/>
-    </row>
-    <row r="1856" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1856" s="1"/>
-    </row>
-    <row r="1857" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1857" s="1"/>
-    </row>
-    <row r="1858" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1858" s="1"/>
-    </row>
-    <row r="1859" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1859" s="1"/>
-    </row>
-    <row r="1860" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1860" s="1"/>
-    </row>
-    <row r="1967" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1967" s="1"/>
-    </row>
-    <row r="1968" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1968" s="1"/>
-    </row>
-    <row r="1969" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1969" s="1"/>
-    </row>
-    <row r="1970" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1970" s="1"/>
-    </row>
-    <row r="1971" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1971" s="1"/>
-    </row>
-    <row r="1972" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1972" s="1"/>
-    </row>
-    <row r="1973" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1973" s="1"/>
-    </row>
-    <row r="1974" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1974" s="1"/>
-    </row>
-    <row r="1975" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1975" s="1"/>
-    </row>
-    <row r="1976" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1976" s="1"/>
-    </row>
-    <row r="1977" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1977" s="1"/>
-    </row>
-    <row r="1978" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1978" s="1"/>
-    </row>
-    <row r="1979" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1979" s="1"/>
-    </row>
-    <row r="1980" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1980" s="1"/>
-    </row>
-    <row r="1981" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1981" s="1"/>
-    </row>
-    <row r="1982" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1982" s="1"/>
-    </row>
-    <row r="1983" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1983" s="1"/>
-    </row>
-    <row r="1984" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1984" s="1"/>
-    </row>
-    <row r="1985" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1985" s="1"/>
-    </row>
-    <row r="1987" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1987" s="1"/>
-    </row>
-    <row r="1990" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1990" s="1"/>
-    </row>
-    <row r="1991" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1991" s="1"/>
-    </row>
-    <row r="1992" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1992" s="1"/>
-    </row>
-    <row r="1993" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F1993" s="1"/>
-    </row>
-    <row r="2033" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2033" s="3"/>
-    </row>
-    <row r="2035" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2035" s="3"/>
-    </row>
-    <row r="2037" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2037" s="3"/>
-    </row>
-    <row r="2038" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2038" s="3"/>
-    </row>
-    <row r="2039" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2039" s="3"/>
-    </row>
-    <row r="2040" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2040" s="3"/>
-    </row>
-    <row r="2041" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2041" s="2"/>
-    </row>
-    <row r="2042" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2042" s="2"/>
-    </row>
-    <row r="2043" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2043" s="2"/>
-    </row>
-    <row r="2044" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2044" s="2"/>
-    </row>
-    <row r="2045" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2045" s="2"/>
-    </row>
-    <row r="2046" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2046" s="2"/>
-    </row>
-    <row r="2047" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2047" s="2"/>
-    </row>
-    <row r="2048" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2048" s="2"/>
-    </row>
-    <row r="2049" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2049" s="2"/>
-    </row>
-    <row r="2050" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2050" s="2"/>
-    </row>
-    <row r="2051" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2051" s="2"/>
-    </row>
-    <row r="2052" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2052" s="2"/>
-    </row>
-    <row r="2053" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2053" s="2"/>
-    </row>
-    <row r="2054" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2054" s="2"/>
-    </row>
-    <row r="2055" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2055" s="2"/>
-    </row>
-    <row r="2056" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2056" s="2"/>
+    <row r="1923" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1923" s="1"/>
+    </row>
+    <row r="1924" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1924" s="1"/>
+    </row>
+    <row r="1925" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1925" s="1"/>
+    </row>
+    <row r="1926" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1926" s="1"/>
+    </row>
+    <row r="1927" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1927" s="1"/>
+    </row>
+    <row r="1928" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1928" s="1"/>
+    </row>
+    <row r="1929" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1929" s="1"/>
+    </row>
+    <row r="1930" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1930" s="1"/>
+    </row>
+    <row r="1931" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1931" s="1"/>
+    </row>
+    <row r="1932" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1932" s="1"/>
+    </row>
+    <row r="1933" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1933" s="1"/>
+    </row>
+    <row r="1934" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1934" s="1"/>
+    </row>
+    <row r="1935" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1935" s="1"/>
+    </row>
+    <row r="1936" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1936" s="1"/>
+    </row>
+    <row r="1937" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1937" s="1"/>
+    </row>
+    <row r="1938" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1938" s="1"/>
+    </row>
+    <row r="1939" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1939" s="1"/>
+    </row>
+    <row r="1940" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1940" s="1"/>
+    </row>
+    <row r="1941" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1941" s="1"/>
+    </row>
+    <row r="1943" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1943" s="1"/>
+    </row>
+    <row r="1946" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1946" s="1"/>
+    </row>
+    <row r="1947" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1947" s="1"/>
+    </row>
+    <row r="1948" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1948" s="1"/>
+    </row>
+    <row r="1949" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F1949" s="1"/>
+    </row>
+    <row r="1989" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1989" s="3"/>
+    </row>
+    <row r="1991" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1991" s="3"/>
+    </row>
+    <row r="1993" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1993" s="3"/>
+    </row>
+    <row r="1994" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1994" s="3"/>
+    </row>
+    <row r="1995" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1995" s="3"/>
+    </row>
+    <row r="1996" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1996" s="3"/>
+    </row>
+    <row r="1997" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1997" s="2"/>
+    </row>
+    <row r="1998" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1998" s="2"/>
+    </row>
+    <row r="1999" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1999" s="2"/>
+    </row>
+    <row r="2000" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2000" s="2"/>
+    </row>
+    <row r="2001" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2001" s="2"/>
+    </row>
+    <row r="2002" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2002" s="2"/>
+    </row>
+    <row r="2003" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2003" s="2"/>
+    </row>
+    <row r="2004" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2004" s="2"/>
+    </row>
+    <row r="2005" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2005" s="2"/>
+    </row>
+    <row r="2006" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2006" s="2"/>
+    </row>
+    <row r="2007" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2007" s="2"/>
+    </row>
+    <row r="2008" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2008" s="2"/>
+    </row>
+    <row r="2009" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2009" s="2"/>
+    </row>
+    <row r="2010" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2010" s="2"/>
+    </row>
+    <row r="2011" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2011" s="2"/>
+    </row>
+    <row r="2012" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2012" s="2"/>
+    </row>
+    <row r="2203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2203" s="2"/>
+    </row>
+    <row r="2239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2239" s="3"/>
+    </row>
+    <row r="2240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2240" s="3"/>
+    </row>
+    <row r="2241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2241" s="2"/>
+    </row>
+    <row r="2242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2242" s="2"/>
+    </row>
+    <row r="2243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2243" s="2"/>
+    </row>
+    <row r="2244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2244" s="2"/>
+    </row>
+    <row r="2245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2245" s="2"/>
+    </row>
+    <row r="2246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2246" s="2"/>
     </row>
     <row r="2247" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2247" s="2"/>
     </row>
-    <row r="2283" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2283" s="3"/>
-    </row>
-    <row r="2284" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2284" s="3"/>
-    </row>
-    <row r="2285" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2285" s="2"/>
-    </row>
-    <row r="2286" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2286" s="2"/>
-    </row>
-    <row r="2287" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2287" s="2"/>
-    </row>
-    <row r="2288" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2288" s="2"/>
-    </row>
-    <row r="2289" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2289" s="2"/>
-    </row>
-    <row r="2290" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2290" s="2"/>
-    </row>
-    <row r="2291" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2291" s="2"/>
-    </row>
-    <row r="2292" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2292" s="2"/>
-    </row>
-    <row r="2293" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2293" s="2"/>
-    </row>
-    <row r="2294" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2294" s="2"/>
-    </row>
-    <row r="2295" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2295" s="2"/>
-    </row>
-    <row r="2296" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2296" s="2"/>
-    </row>
-    <row r="2297" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2297" s="2"/>
-    </row>
-    <row r="2298" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2298" s="2"/>
-    </row>
-    <row r="2299" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2299" s="2"/>
-    </row>
-    <row r="2300" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2300" s="2"/>
-    </row>
-    <row r="2301" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2301" s="2"/>
-    </row>
-    <row r="2302" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2302" s="2"/>
-    </row>
-    <row r="2303" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2303" s="2"/>
-    </row>
-    <row r="2304" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2304" s="2"/>
-    </row>
-    <row r="2305" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2305" s="2"/>
-    </row>
-    <row r="2306" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2306" s="2"/>
-    </row>
-    <row r="2307" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2307" s="2"/>
-    </row>
-    <row r="2308" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2308" s="2"/>
-    </row>
-    <row r="2309" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2309" s="2"/>
-    </row>
-    <row r="2310" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2310" s="2"/>
-    </row>
-    <row r="2311" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2311" s="2"/>
-    </row>
-    <row r="2312" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2312" s="2"/>
-    </row>
-    <row r="2313" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2313" s="2"/>
-    </row>
-    <row r="2314" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2314" s="2"/>
-    </row>
-    <row r="2315" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2315" s="2"/>
-    </row>
-    <row r="2316" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2316" s="2"/>
-    </row>
-    <row r="2317" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2317" s="2"/>
-    </row>
-    <row r="2318" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2318" s="2"/>
-    </row>
-    <row r="2319" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2319" s="2"/>
-    </row>
-    <row r="2320" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2320" s="2"/>
-    </row>
-    <row r="2321" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2321" s="2"/>
-    </row>
-    <row r="2381" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2381" s="2"/>
-    </row>
-    <row r="2382" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2382" s="2"/>
-    </row>
-    <row r="2383" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2383" s="2"/>
-    </row>
-    <row r="2384" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2384" s="2"/>
-    </row>
-    <row r="2385" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2385" s="2"/>
-    </row>
-    <row r="2386" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2386" s="2"/>
-    </row>
-    <row r="2387" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2387" s="2"/>
-    </row>
-    <row r="2388" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2388" s="2"/>
-    </row>
-    <row r="2389" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2389" s="2"/>
-    </row>
-    <row r="2390" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2390" s="2"/>
-    </row>
-    <row r="2391" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2391" s="2"/>
-    </row>
-    <row r="2392" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2392" s="2"/>
-    </row>
-    <row r="2393" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2393" s="2"/>
+    <row r="2248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2248" s="2"/>
+    </row>
+    <row r="2249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2249" s="2"/>
+    </row>
+    <row r="2250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2250" s="2"/>
+    </row>
+    <row r="2251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2251" s="2"/>
+    </row>
+    <row r="2252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2252" s="2"/>
+    </row>
+    <row r="2253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2253" s="2"/>
+    </row>
+    <row r="2254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2254" s="2"/>
+    </row>
+    <row r="2255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2255" s="2"/>
+    </row>
+    <row r="2256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2256" s="2"/>
+    </row>
+    <row r="2257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2257" s="2"/>
+    </row>
+    <row r="2258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2258" s="2"/>
+    </row>
+    <row r="2259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2259" s="2"/>
+    </row>
+    <row r="2260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2260" s="2"/>
+    </row>
+    <row r="2261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2261" s="2"/>
+    </row>
+    <row r="2262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2262" s="2"/>
+    </row>
+    <row r="2263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2263" s="2"/>
+    </row>
+    <row r="2264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2264" s="2"/>
+    </row>
+    <row r="2265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2265" s="2"/>
+    </row>
+    <row r="2266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2266" s="2"/>
+    </row>
+    <row r="2267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2267" s="2"/>
+    </row>
+    <row r="2268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2268" s="2"/>
+    </row>
+    <row r="2269" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2269" s="2"/>
+    </row>
+    <row r="2270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2270" s="2"/>
+    </row>
+    <row r="2271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2271" s="2"/>
+    </row>
+    <row r="2272" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2272" s="2"/>
+    </row>
+    <row r="2273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2273" s="2"/>
+    </row>
+    <row r="2274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2274" s="2"/>
+    </row>
+    <row r="2275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2275" s="2"/>
+    </row>
+    <row r="2276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2276" s="2"/>
+    </row>
+    <row r="2277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2277" s="2"/>
+    </row>
+    <row r="2337" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2337" s="2"/>
+    </row>
+    <row r="2338" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2338" s="2"/>
+    </row>
+    <row r="2339" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2339" s="2"/>
+    </row>
+    <row r="2340" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2340" s="2"/>
+    </row>
+    <row r="2341" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2341" s="2"/>
+    </row>
+    <row r="2342" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2342" s="2"/>
+    </row>
+    <row r="2343" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2343" s="2"/>
+    </row>
+    <row r="2344" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2344" s="2"/>
+    </row>
+    <row r="2345" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2345" s="2"/>
+    </row>
+    <row r="2346" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2346" s="2"/>
+    </row>
+    <row r="2347" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2347" s="2"/>
+    </row>
+    <row r="2348" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2348" s="2"/>
+    </row>
+    <row r="2349" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2349" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>